<commit_message>
Improve mapbox visualization and add testset
</commit_message>
<xml_diff>
--- a/data/10years.testset.xlsx
+++ b/data/10years.testset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="231">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Casualty description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casualty count</t>
   </si>
   <si>
     <t xml:space="preserve">Regions</t>
@@ -826,12 +829,12 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
+      <selection pane="bottomLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="1" style="1" width="20.71"/>
   </cols>
@@ -853,114 +856,114 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>40</v>
@@ -968,782 +971,782 @@
     </row>
     <row r="9" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>15</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>185</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>6</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>24</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F39" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update testset xlsx file
</commit_message>
<xml_diff>
--- a/data/10years.testset.xlsx
+++ b/data/10years.testset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="205">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -49,6 +49,12 @@
     <t xml:space="preserve">Terrorism in Bangladesh: Raids by security forces on Jamaat-ul-Mujahideen Bangladesh in Gazipur leave 11 militants dead. (The Hindustan Times), (Reuters), (The Voice of America News)</t>
   </si>
   <si>
+    <t xml:space="preserve">Valid Accurate Incomplete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Accurate Complete</t>
+  </si>
+  <si>
     <t xml:space="preserve">BGD</t>
   </si>
   <si>
@@ -295,6 +301,9 @@
     <t xml:space="preserve">Iraqi Civil War (2014–2017): 2017 Western Iraq campaign: Mass graves containing at least 400 bodies have been found near Hawija, an Iraqi city that was occupied by ISIL until last month. (BBC)</t>
   </si>
   <si>
+    <t xml:space="preserve">Invalid Accurate Incomplete</t>
+  </si>
+  <si>
     <t xml:space="preserve">2010-08-18-8e01da</t>
   </si>
   <si>
@@ -382,6 +391,9 @@
     <t xml:space="preserve">NGA</t>
   </si>
   <si>
+    <t xml:space="preserve">Invalid Inaccurate Complete</t>
+  </si>
+  <si>
     <t xml:space="preserve">11.5, 13.0</t>
   </si>
   <si>
@@ -427,9 +439,15 @@
     <t xml:space="preserve">Boko Haram insurgency: A suicide bombing kills at least 24 people at a mosque in Mubi, Nigeria. Boko Haram are suspected of being behind the attack. (BBC)</t>
   </si>
   <si>
+    <t xml:space="preserve">Invalid Accurate Complete</t>
+  </si>
+  <si>
     <t xml:space="preserve">at least 24 people at a mosque in Mubi, Nigeria. Boko Haram are suspected of being behind the attack. (BBC</t>
   </si>
   <si>
+    <t xml:space="preserve">Valid Inaccurate Complete</t>
+  </si>
+  <si>
     <t xml:space="preserve">CMR, NER, NGA</t>
   </si>
   <si>
@@ -598,15 +616,6 @@
     <t xml:space="preserve">36.0, 128.0</t>
   </si>
   <si>
-    <t xml:space="preserve">2016-09-29-88acaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syrian Civil War: A video from besieged eastern Aleppo's al-Shaar neighborhood emerges showing the moment a young girl, identified as Ghazal Qasim, trapped beneath rubble of a five floor building blown to smithereens by a deadly Assad government's bunker buster bomb attack on September 27, is rescued by the Syrian Civil Defense, better known as the white helmets. (International Business Times)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36.2, 37.15</t>
-  </si>
-  <si>
     <t xml:space="preserve">2011-08-22-053735</t>
   </si>
   <si>
@@ -619,100 +628,13 @@
     <t xml:space="preserve">-29.0, 24.0</t>
   </si>
   <si>
-    <t xml:space="preserve">2012-02-21-74c5c0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rioting inmates take control of Indonesia's Kerobokan Prison on the island of Bali. (Sydney Morning Herald)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8.5, 115.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8.67277778, 115.16805556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.0, 118.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-06-17-7449e7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boko Haram: Boko Haram terrorists exchange gunfire with Nigerian troops in the Nganzai local government area of Borno State. (Al Jazeera)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGA, CMR, NER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.508888888, 13.104166666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.486253, 13.209321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011-05-02-217acc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libyan Civil War: The United Nations withdraws all of its international staff from the capital Tripoli. (BBC) (Al Jazeera)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LBY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32.87519, 13.18746</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-07-26-fb9df4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016 Normandy church attack: Following the murder of the Catholic priest, French President François Hollande vows to wage war against the Islamic State of Iraq and the Levant "by every means". The organization released a video showing the attackers pledging allegiance to ISIL during the attack. (Local)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.380305, 1.108209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011-01-15-a94d0b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010–2011 Tunisian protests: Saudi Arabia confirms it is welcoming ousted Zine El Abidine Ben Ali and his family into the kingdom due to "exceptional circumstances" in Tunisia; people in Saudi Arabia and people elsewhere criticise the decision to offer sanctuary to "the dictator" on the Internet. (Al Jazeera) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAU, TUN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.0, 10.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-11-11-e9cea7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syrian Civil War, Spillover of the Syrian Civil War: The Israeli Air Force reportedly conducts an airstrike near Damascus International Airport, in Syria's capital, the target apparently a weapons shipment reportedly intended for Lebanese terrorist organization Hezbollah, according to Syrian opposition groups. (Times of Israel) (The Jerusalem Post)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISR, SYR, LBN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36.0, 37.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.411522222, 36.515558333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014-06-16-ac6af0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014 Northern Iraq offensive: The Pentagon sends the USS Mesa Verde to the Persian Gulf to join a contingency of U.S. Navy ships already stationed there to monitor the northern offensive. (NBC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRQ, SYR, USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.0, 52.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36.337222222, 43.135833333</t>
+    <t xml:space="preserve">Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accurate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete</t>
   </si>
 </sst>
 </file>
@@ -762,11 +684,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -796,7 +725,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -807,6 +736,30 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -826,17 +779,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="1" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="1" width="21.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="13" style="1" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,894 +832,1493 @@
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>15</v>
       </c>
+      <c r="G21" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H21" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G32" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H32" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>185</v>
       </c>
+      <c r="G33" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H33" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="G35" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H35" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>24</v>
       </c>
+      <c r="G36" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="H36" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F39" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="5" t="n">
         <v>1</v>
       </c>
+      <c r="G39" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H39" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>155</v>
+        <v>161</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G41" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H41" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>169</v>
+        <v>175</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>178</v>
+        <v>184</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>186</v>
+        <v>192</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>189</v>
+        <v>195</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>36</v>
+        <v>200</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7" t="n">
+        <f aca="false">ROWS(C2:C51) - (COUNTIF(C2:C51,"*invalid*"))</f>
+        <v>49</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E52" s="7" t="n">
+        <f aca="false">ROWS(E2:E51) - (COUNTIF(E2:E51,"*invalid*"))</f>
+        <v>49</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G52" s="7" t="n">
+        <f aca="false">ROWS(G2:G51) - (COUNTIF(G2:G51,"*invalid*"))</f>
+        <v>49</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="I52" s="7" t="n">
+        <f aca="false">ROWS(I2:I51) - (COUNTIF(I2:I51,"*invalid*"))</f>
+        <v>48</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8" t="n">
+        <f aca="false">ROWS(C2:C51) - COUNTIF(C2:C51,"*inaccurate*")</f>
+        <v>50</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E53" s="8" t="n">
+        <f aca="false">ROWS(E2:E51) - COUNTIF(E2:E51,"*inaccurate*")</f>
+        <v>49</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G53" s="8" t="n">
+        <f aca="false">ROWS(G2:G51) - COUNTIF(G2:G51,"*inaccurate*")</f>
+        <v>48</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
+      </c>
+      <c r="I53" s="8" t="n">
+        <f aca="false">ROWS(I2:I51) - COUNTIF(I2:I51,"*inaccurate*")</f>
+        <v>48</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K53" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L53" s="1" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8" t="n">
+        <f aca="false">ROWS(C2:C51) - COUNTIF(C2:C51,"*incomplete")</f>
+        <v>35</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>206</v>
+      <c r="E54" s="8" t="n">
+        <f aca="false">ROWS(E2:E51) - COUNTIF(E2:E51,"*incomplete")</f>
+        <v>34</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G54" s="8" t="n">
+        <f aca="false">ROWS(G2:G51) - COUNTIF(G2:G51,"*incomplete")</f>
+        <v>34</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
+      </c>
+      <c r="I54" s="8" t="n">
+        <f aca="false">ROWS(I2:I51) - COUNTIF(I2:I51,"*incomplete")</f>
+        <v>33</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="200" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8" t="n">
+        <f aca="false">COUNTIF(C2:C51,"Valid Accurate Complete")</f>
+        <v>34</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="8" t="n">
+        <f aca="false">COUNTIF(E2:E51,"Valid Accurate Complete")</f>
+        <v>33</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="8" t="n">
+        <f aca="false">COUNTIF(G2:G51,"Valid Accurate Complete")</f>
+        <v>32</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="8" t="n">
+        <f aca="false">COUNTIF(I2:I51,"Valid Accurate Complete")</f>
+        <v>31</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C59" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6:C8 E7:E8 G9:G13 I9 C11 E11 I11:I13 G15 I15 C16:C51 E16:E38 G17:G18 I17:I18 G20:G35 I20:I32 I34:I35 I37:I42 G38:G42 E40:E51 G44 I44 G47:G48 I47:I48 G50:G51 I50:I51 B55 D55 F55 H55 J55" type="list">
       <formula1>"Valid Accurate Complete,Invalid Accurate Complete,Valid Inaccurate Complete,Invalid Inaccurate Complete,Valid Accurate Incomplete,Invalid Accurate Incomplete,Valid Inaccurate Incomplete,Invalid Inaccurate Incomplete"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E59" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E6 E39" type="list">
       <formula1>"Valid Accurate Complete,Invalid Accurate Complete,Valid Inaccurate Complete,Invalid Inaccurate Complete,Valid Accurate Incomplete,Invalid Accurate Incomplete,Valid Inaccurate Incomplete,Invalid Inaccurate Incomplete"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G59" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C5 E2:E5 G2:G7 I6 G8 I8 C9:C10 E9:E10 I10 C12:C15 E12:E15 G14 I14 G16 I16 G19 I19 G36:G37 I36 G43 I43 G45:G46 I45:I46 G49 I49" type="list">
       <formula1>"Valid Accurate Complete,Invalid Accurate Complete,Valid Inaccurate Complete,Invalid Inaccurate Complete,Valid Accurate Incomplete,Invalid Accurate Incomplete,Valid Inaccurate Incomplete,Invalid Inaccurate Incomplete"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I59" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I5 I7 I33" type="list">
       <formula1>"Valid Accurate Complete,Invalid Accurate Complete,Valid Inaccurate Complete,Invalid Inaccurate Complete,Valid Accurate Incomplete,Invalid Accurate Incomplete,Valid Inaccurate Incomplete,Invalid Inaccurate Incomplete"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1877,32 +2430,8 @@
     <hyperlink ref="A50" r:id="rId104" display="2011-06-18-7ac467"/>
     <hyperlink ref="J50" r:id="rId105" display="40.0, 127.0"/>
     <hyperlink ref="K50" r:id="rId106" display="36.0, 128.0"/>
-    <hyperlink ref="A51" r:id="rId107" display="2016-09-29-88acaf"/>
-    <hyperlink ref="J51" r:id="rId108" display="36.2, 37.15"/>
-    <hyperlink ref="A52" r:id="rId109" display="2011-08-22-053735"/>
-    <hyperlink ref="J52" r:id="rId110" display="-29.0, 24.0"/>
-    <hyperlink ref="A53" r:id="rId111" display="2012-02-21-74c5c0"/>
-    <hyperlink ref="J53" r:id="rId112" display="-8.5, 115.0"/>
-    <hyperlink ref="K53" r:id="rId113" display="-8.67277778, 115.16805556"/>
-    <hyperlink ref="L53" r:id="rId114" display="-2.0, 118.0"/>
-    <hyperlink ref="A54" r:id="rId115" display="2019-06-17-7449e7"/>
-    <hyperlink ref="J54" r:id="rId116" display="12.508888888, 13.104166666"/>
-    <hyperlink ref="K54" r:id="rId117" display="12.486253, 13.209321"/>
-    <hyperlink ref="A55" r:id="rId118" display="2011-05-02-217acc"/>
-    <hyperlink ref="J55" r:id="rId119" display="32.87519, 13.18746"/>
-    <hyperlink ref="A56" r:id="rId120" display="2016-07-26-fb9df4"/>
-    <hyperlink ref="J56" r:id="rId121" display="49.380305, 1.108209"/>
-    <hyperlink ref="A57" r:id="rId122" display="2011-01-15-a94d0b"/>
-    <hyperlink ref="J57" r:id="rId123" display="23.716667, 44.116667"/>
-    <hyperlink ref="K57" r:id="rId124" display="34.0, 10.0"/>
-    <hyperlink ref="A58" r:id="rId125" display="2015-11-11-e9cea7"/>
-    <hyperlink ref="J58" r:id="rId126" display="36.0, 37.0"/>
-    <hyperlink ref="K58" r:id="rId127" display="33.411522222, 36.515558333"/>
-    <hyperlink ref="L58" r:id="rId128" display="33.833333, 35.766667"/>
-    <hyperlink ref="M58" r:id="rId129" display="35.216667, 38.583333"/>
-    <hyperlink ref="A59" r:id="rId130" display="2014-06-16-ac6af0"/>
-    <hyperlink ref="J59" r:id="rId131" display="26.0, 52.0"/>
-    <hyperlink ref="K59" r:id="rId132" display="36.337222222, 43.135833333"/>
+    <hyperlink ref="A51" r:id="rId107" display="2011-08-22-053735"/>
+    <hyperlink ref="J51" r:id="rId108" display="-29.0, 24.0"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>